<commit_message>
Got the square cards building with correct size
</commit_message>
<xml_diff>
--- a/data/disturbance-deck.xlsx
+++ b/data/disturbance-deck.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathan.jones\Documents\GitHub\Raspberry\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Raspberry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>BaseType</t>
   </si>
@@ -92,9 +92,6 @@
     <t>:W: :W:</t>
   </si>
   <si>
-    <t>If discovered by a player that's not in the same space, flip this face down.</t>
-  </si>
-  <si>
     <t>Healer's Care</t>
   </si>
   <si>
@@ -102,12 +99,27 @@
   </si>
   <si>
     <t>Lose 3 :heart:</t>
+  </si>
+  <si>
+    <t>horror</t>
+  </si>
+  <si>
+    <t>Sewer Tentacles</t>
+  </si>
+  <si>
+    <t>:H: :H:</t>
+  </si>
+  <si>
+    <t>If revealed by a player that's not in the same space, flip this face down.</t>
+  </si>
+  <si>
+    <t>When revealed, all players on the edge of the city lose 2 :heart:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,10 +527,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -532,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -623,7 +635,27 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added combat dice to disturbance cards
</commit_message>
<xml_diff>
--- a/data/disturbance-deck.xlsx
+++ b/data/disturbance-deck.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Raspberry\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Projects\Raspberry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -107,19 +107,19 @@
     <t>Sewer Tentacles</t>
   </si>
   <si>
-    <t>:H: :H:</t>
-  </si>
-  <si>
     <t>If revealed by a player that's not in the same space, flip this face down.</t>
   </si>
   <si>
     <t>When revealed, all players on the edge of the city lose 2 :heart:</t>
+  </si>
+  <si>
+    <t>:G: :G:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -652,10 +652,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to support player cards for hunt the beast
Also added a basic rules document
</commit_message>
<xml_diff>
--- a/data/disturbance-deck.xlsx
+++ b/data/disturbance-deck.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Projects\Raspberry\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Google Drive\Projects\Raspberry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>BaseType</t>
   </si>
@@ -47,15 +48,6 @@
     <t>event</t>
   </si>
   <si>
-    <t>Horrific Scene</t>
-  </si>
-  <si>
-    <t>Gain 1 :corruption: and reveal the next Doom card</t>
-  </si>
-  <si>
-    <t>Rotting Shambler</t>
-  </si>
-  <si>
     <t>zombie</t>
   </si>
   <si>
@@ -65,30 +57,15 @@
     <t>Spring Trap</t>
   </si>
   <si>
-    <t>Skinface</t>
-  </si>
-  <si>
-    <t>Sprinting Corpse</t>
-  </si>
-  <si>
     <t>:R: :R:</t>
   </si>
   <si>
-    <t>When discovered, move this to your square.  This fights you immediately.</t>
-  </si>
-  <si>
     <t>lychenthrope</t>
   </si>
   <si>
-    <t>Emaciated Wererat</t>
-  </si>
-  <si>
     <t>:W:</t>
   </si>
   <si>
-    <t>Toothy Little Girl</t>
-  </si>
-  <si>
     <t>:W: :W:</t>
   </si>
   <si>
@@ -104,13 +81,70 @@
     <t>horror</t>
   </si>
   <si>
-    <t>Sewer Tentacles</t>
-  </si>
-  <si>
-    <t>If revealed by a player that's not in the same space, flip this face down.</t>
-  </si>
-  <si>
-    <t>When revealed, all players on the edge of the city lose 2 :heart:</t>
+    <t>Small Zombie</t>
+  </si>
+  <si>
+    <t>Large Zombie</t>
+  </si>
+  <si>
+    <t>Small Lychenthrope</t>
+  </si>
+  <si>
+    <t>Large Lychenthrope</t>
+  </si>
+  <si>
+    <t>Horror</t>
+  </si>
+  <si>
+    <t>Gain 1 :corruption:</t>
+  </si>
+  <si>
+    <t>Gain 1 :corruption:
+All players gain 3 :coin:</t>
+  </si>
+  <si>
+    <t>Gain 3 :heart:
+or
+All players gain 1 :heart:</t>
+  </si>
+  <si>
+    <t>Learn a Lesson</t>
+  </si>
+  <si>
+    <t>Each player draws the top card of the Purchase deck</t>
+  </si>
+  <si>
+    <t>Receive Exorcism</t>
+  </si>
+  <si>
+    <t>Discover Horrific Scene</t>
+  </si>
+  <si>
+    <t>Remove 2 Corruption cards from your deck and / or discard pile.  Then shuffle your deck.</t>
+  </si>
+  <si>
+    <t>Murder of Crows</t>
+  </si>
+  <si>
+    <t>Reveal the next Doom card</t>
+  </si>
+  <si>
+    <t>Gossip Among Villiagers</t>
+  </si>
+  <si>
+    <t>Reveal any Disturbance in the City</t>
+  </si>
+  <si>
+    <t>Find Cache of Goods</t>
+  </si>
+  <si>
+    <t>Gain 3 :coin:</t>
+  </si>
+  <si>
+    <t>Eat Hearty Meal</t>
+  </si>
+  <si>
+    <t>Tainted Blessing</t>
   </si>
   <si>
     <t>:G: :G:</t>
@@ -119,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -468,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,157 +539,229 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="1">
-        <v>4</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>